<commit_message>
Moved Reusable back into Book Flights
</commit_message>
<xml_diff>
--- a/Book Flights/Default.xlsx
+++ b/Book Flights/Default.xlsx
@@ -1013,16 +1013,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1330,9 +1330,9 @@
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="11.7109375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" style="5" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" style="6" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" style="3" customWidth="1"/>
-    <col min="4" max="255" width="9.140625" style="5" customWidth="1"/>
+    <col min="4" max="255" width="9.140625" style="6" customWidth="1"/>
     <col min="256" max="16384" width="9.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2107,7 +2107,7 @@
       <c s="4" t="s">
         <v>205</v>
       </c>
-      <c s="7" t="s">
+      <c s="8" t="s">
         <v>74</v>
       </c>
       <c s="4" t="s">
@@ -2364,13 +2364,13 @@
       <c s="1"/>
       <c s="1"/>
       <c s="1"/>
-      <c s="8"/>
+      <c s="7"/>
     </row>
     <row s="2" customFormat="1">
       <c s="4" t="s">
         <v>0</v>
       </c>
-      <c s="7" t="s">
+      <c s="8" t="s">
         <v>205</v>
       </c>
       <c s="4"/>
@@ -2625,13 +2625,13 @@
       <c s="1"/>
       <c s="1"/>
       <c s="1"/>
-      <c s="8"/>
+      <c s="7"/>
     </row>
     <row s="2" customFormat="1">
       <c s="4" t="s">
         <v>244</v>
       </c>
-      <c s="7" t="s">
+      <c s="8" t="s">
         <v>89</v>
       </c>
       <c s="4"/>
@@ -2886,13 +2886,13 @@
       <c s="1"/>
       <c s="1"/>
       <c s="1"/>
-      <c s="8"/>
+      <c s="7"/>
     </row>
     <row s="2" customFormat="1">
       <c s="4" t="s">
         <v>89</v>
       </c>
-      <c s="7" t="s">
+      <c s="8" t="s">
         <v>244</v>
       </c>
       <c s="4"/>
@@ -3147,7 +3147,7 @@
       <c s="1"/>
       <c s="1"/>
       <c s="1"/>
-      <c s="8"/>
+      <c s="7"/>
     </row>
   </sheetData>
   <printOptions gridLines="1"/>
@@ -3259,7 +3259,7 @@
       <c s="4" t="s">
         <v>45</v>
       </c>
-      <c s="6" t="str">
+      <c s="5" t="str">
         <f>"DSN=Flights;Database=C:\Users\"&amp;A2&amp;"\AppData\Local\UFT\Demo\DB\Flights.s3db;StepAPI=0;SyncPragma=;NoTXN=0;Timeout=;ShortNames=0;LongNames=0;NoCreat=0;NoWCHAR=0;FKSupport=0;JournalMode=;OEMCP=0;LoadExt=;BigInt=0;JDConv=0;PWD="</f>
         <v>DSN=Flights;Database=C:\Users\someone\AppData\Local\UFT\Demo\DB\Flights.s3db;StepAPI=0;SyncPragma=;NoTXN=0;Timeout=;ShortNames=0;LongNames=0;NoCreat=0;NoWCHAR=0;FKSupport=0;JournalMode=;OEMCP=0;LoadExt=;BigInt=0;JDConv=0;PWD=</v>
       </c>
@@ -3301,7 +3301,7 @@
       <c s="1" t="s">
         <v>65</v>
       </c>
-      <c s="6" t="str">
+      <c s="5" t="str">
         <f t="shared" si="0" ref="B2:B8">"DSN=Flights;Database=C:\Users\"&amp;A2&amp;"\AppData\Local\UFT\Demo\DB\Flights.s3db;StepAPI=0;SyncPragma=;NoTXN=0;Timeout=;ShortNames=0;LongNames=0;NoCreat=0;NoWCHAR=0;FKSupport=0;JournalMode=;OEMCP=0;LoadExt=;BigInt=0;JDConv=0;PWD="</f>
         <v>DSN=Flights;Database=C:\Users\somone\AppData\Local\UFT\Demo\DB\Flights.s3db;StepAPI=0;SyncPragma=;NoTXN=0;Timeout=;ShortNames=0;LongNames=0;NoCreat=0;NoWCHAR=0;FKSupport=0;JournalMode=;OEMCP=0;LoadExt=;BigInt=0;JDConv=0;PWD=</v>
       </c>
@@ -3310,7 +3310,7 @@
       <c s="1" t="s">
         <v>65</v>
       </c>
-      <c s="6" t="str">
+      <c s="5" t="str">
         <f t="shared" si="0"/>
         <v>DSN=Flights;Database=C:\Users\somone\AppData\Local\UFT\Demo\DB\Flights.s3db;StepAPI=0;SyncPragma=;NoTXN=0;Timeout=;ShortNames=0;LongNames=0;NoCreat=0;NoWCHAR=0;FKSupport=0;JournalMode=;OEMCP=0;LoadExt=;BigInt=0;JDConv=0;PWD=</v>
       </c>
@@ -3319,7 +3319,7 @@
       <c s="1" t="s">
         <v>65</v>
       </c>
-      <c s="6" t="str">
+      <c s="5" t="str">
         <f t="shared" si="0"/>
         <v>DSN=Flights;Database=C:\Users\somone\AppData\Local\UFT\Demo\DB\Flights.s3db;StepAPI=0;SyncPragma=;NoTXN=0;Timeout=;ShortNames=0;LongNames=0;NoCreat=0;NoWCHAR=0;FKSupport=0;JournalMode=;OEMCP=0;LoadExt=;BigInt=0;JDConv=0;PWD=</v>
       </c>
@@ -3328,7 +3328,7 @@
       <c s="1" t="s">
         <v>65</v>
       </c>
-      <c s="6" t="str">
+      <c s="5" t="str">
         <f t="shared" si="0"/>
         <v>DSN=Flights;Database=C:\Users\somone\AppData\Local\UFT\Demo\DB\Flights.s3db;StepAPI=0;SyncPragma=;NoTXN=0;Timeout=;ShortNames=0;LongNames=0;NoCreat=0;NoWCHAR=0;FKSupport=0;JournalMode=;OEMCP=0;LoadExt=;BigInt=0;JDConv=0;PWD=</v>
       </c>
@@ -3337,7 +3337,7 @@
       <c s="1" t="s">
         <v>65</v>
       </c>
-      <c s="6" t="str">
+      <c s="5" t="str">
         <f t="shared" si="0"/>
         <v>DSN=Flights;Database=C:\Users\somone\AppData\Local\UFT\Demo\DB\Flights.s3db;StepAPI=0;SyncPragma=;NoTXN=0;Timeout=;ShortNames=0;LongNames=0;NoCreat=0;NoWCHAR=0;FKSupport=0;JournalMode=;OEMCP=0;LoadExt=;BigInt=0;JDConv=0;PWD=</v>
       </c>
@@ -3346,7 +3346,7 @@
       <c s="1" t="s">
         <v>65</v>
       </c>
-      <c s="6" t="str">
+      <c s="5" t="str">
         <f t="shared" si="0"/>
         <v>DSN=Flights;Database=C:\Users\somone\AppData\Local\UFT\Demo\DB\Flights.s3db;StepAPI=0;SyncPragma=;NoTXN=0;Timeout=;ShortNames=0;LongNames=0;NoCreat=0;NoWCHAR=0;FKSupport=0;JournalMode=;OEMCP=0;LoadExt=;BigInt=0;JDConv=0;PWD=</v>
       </c>
@@ -3355,7 +3355,7 @@
       <c s="1" t="s">
         <v>65</v>
       </c>
-      <c s="6" t="str">
+      <c s="5" t="str">
         <f t="shared" si="0"/>
         <v>DSN=Flights;Database=C:\Users\somone\AppData\Local\UFT\Demo\DB\Flights.s3db;StepAPI=0;SyncPragma=;NoTXN=0;Timeout=;ShortNames=0;LongNames=0;NoCreat=0;NoWCHAR=0;FKSupport=0;JournalMode=;OEMCP=0;LoadExt=;BigInt=0;JDConv=0;PWD=</v>
       </c>

</xml_diff>

<commit_message>
Changed Reusable folder back to top and used ..\Reusable
</commit_message>
<xml_diff>
--- a/Book Flights/Default.xlsx
+++ b/Book Flights/Default.xlsx
@@ -1013,16 +1013,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1330,9 +1330,9 @@
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="11.7109375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" style="6" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" style="5" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" style="3" customWidth="1"/>
-    <col min="4" max="255" width="9.140625" style="6" customWidth="1"/>
+    <col min="4" max="255" width="9.140625" style="5" customWidth="1"/>
     <col min="256" max="16384" width="9.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2107,7 +2107,7 @@
       <c s="4" t="s">
         <v>205</v>
       </c>
-      <c s="8" t="s">
+      <c s="7" t="s">
         <v>74</v>
       </c>
       <c s="4" t="s">
@@ -2364,13 +2364,13 @@
       <c s="1"/>
       <c s="1"/>
       <c s="1"/>
-      <c s="7"/>
+      <c s="8"/>
     </row>
     <row s="2" customFormat="1">
       <c s="4" t="s">
         <v>0</v>
       </c>
-      <c s="8" t="s">
+      <c s="7" t="s">
         <v>205</v>
       </c>
       <c s="4"/>
@@ -2625,13 +2625,13 @@
       <c s="1"/>
       <c s="1"/>
       <c s="1"/>
-      <c s="7"/>
+      <c s="8"/>
     </row>
     <row s="2" customFormat="1">
       <c s="4" t="s">
         <v>244</v>
       </c>
-      <c s="8" t="s">
+      <c s="7" t="s">
         <v>89</v>
       </c>
       <c s="4"/>
@@ -2886,13 +2886,13 @@
       <c s="1"/>
       <c s="1"/>
       <c s="1"/>
-      <c s="7"/>
+      <c s="8"/>
     </row>
     <row s="2" customFormat="1">
       <c s="4" t="s">
         <v>89</v>
       </c>
-      <c s="8" t="s">
+      <c s="7" t="s">
         <v>244</v>
       </c>
       <c s="4"/>
@@ -3147,7 +3147,7 @@
       <c s="1"/>
       <c s="1"/>
       <c s="1"/>
-      <c s="7"/>
+      <c s="8"/>
     </row>
   </sheetData>
   <printOptions gridLines="1"/>
@@ -3259,7 +3259,7 @@
       <c s="4" t="s">
         <v>45</v>
       </c>
-      <c s="5" t="str">
+      <c s="6" t="str">
         <f>"DSN=Flights;Database=C:\Users\"&amp;A2&amp;"\AppData\Local\UFT\Demo\DB\Flights.s3db;StepAPI=0;SyncPragma=;NoTXN=0;Timeout=;ShortNames=0;LongNames=0;NoCreat=0;NoWCHAR=0;FKSupport=0;JournalMode=;OEMCP=0;LoadExt=;BigInt=0;JDConv=0;PWD="</f>
         <v>DSN=Flights;Database=C:\Users\someone\AppData\Local\UFT\Demo\DB\Flights.s3db;StepAPI=0;SyncPragma=;NoTXN=0;Timeout=;ShortNames=0;LongNames=0;NoCreat=0;NoWCHAR=0;FKSupport=0;JournalMode=;OEMCP=0;LoadExt=;BigInt=0;JDConv=0;PWD=</v>
       </c>
@@ -3301,7 +3301,7 @@
       <c s="1" t="s">
         <v>65</v>
       </c>
-      <c s="5" t="str">
+      <c s="6" t="str">
         <f t="shared" si="0" ref="B2:B8">"DSN=Flights;Database=C:\Users\"&amp;A2&amp;"\AppData\Local\UFT\Demo\DB\Flights.s3db;StepAPI=0;SyncPragma=;NoTXN=0;Timeout=;ShortNames=0;LongNames=0;NoCreat=0;NoWCHAR=0;FKSupport=0;JournalMode=;OEMCP=0;LoadExt=;BigInt=0;JDConv=0;PWD="</f>
         <v>DSN=Flights;Database=C:\Users\somone\AppData\Local\UFT\Demo\DB\Flights.s3db;StepAPI=0;SyncPragma=;NoTXN=0;Timeout=;ShortNames=0;LongNames=0;NoCreat=0;NoWCHAR=0;FKSupport=0;JournalMode=;OEMCP=0;LoadExt=;BigInt=0;JDConv=0;PWD=</v>
       </c>
@@ -3310,7 +3310,7 @@
       <c s="1" t="s">
         <v>65</v>
       </c>
-      <c s="5" t="str">
+      <c s="6" t="str">
         <f t="shared" si="0"/>
         <v>DSN=Flights;Database=C:\Users\somone\AppData\Local\UFT\Demo\DB\Flights.s3db;StepAPI=0;SyncPragma=;NoTXN=0;Timeout=;ShortNames=0;LongNames=0;NoCreat=0;NoWCHAR=0;FKSupport=0;JournalMode=;OEMCP=0;LoadExt=;BigInt=0;JDConv=0;PWD=</v>
       </c>
@@ -3319,7 +3319,7 @@
       <c s="1" t="s">
         <v>65</v>
       </c>
-      <c s="5" t="str">
+      <c s="6" t="str">
         <f t="shared" si="0"/>
         <v>DSN=Flights;Database=C:\Users\somone\AppData\Local\UFT\Demo\DB\Flights.s3db;StepAPI=0;SyncPragma=;NoTXN=0;Timeout=;ShortNames=0;LongNames=0;NoCreat=0;NoWCHAR=0;FKSupport=0;JournalMode=;OEMCP=0;LoadExt=;BigInt=0;JDConv=0;PWD=</v>
       </c>
@@ -3328,7 +3328,7 @@
       <c s="1" t="s">
         <v>65</v>
       </c>
-      <c s="5" t="str">
+      <c s="6" t="str">
         <f t="shared" si="0"/>
         <v>DSN=Flights;Database=C:\Users\somone\AppData\Local\UFT\Demo\DB\Flights.s3db;StepAPI=0;SyncPragma=;NoTXN=0;Timeout=;ShortNames=0;LongNames=0;NoCreat=0;NoWCHAR=0;FKSupport=0;JournalMode=;OEMCP=0;LoadExt=;BigInt=0;JDConv=0;PWD=</v>
       </c>
@@ -3337,7 +3337,7 @@
       <c s="1" t="s">
         <v>65</v>
       </c>
-      <c s="5" t="str">
+      <c s="6" t="str">
         <f t="shared" si="0"/>
         <v>DSN=Flights;Database=C:\Users\somone\AppData\Local\UFT\Demo\DB\Flights.s3db;StepAPI=0;SyncPragma=;NoTXN=0;Timeout=;ShortNames=0;LongNames=0;NoCreat=0;NoWCHAR=0;FKSupport=0;JournalMode=;OEMCP=0;LoadExt=;BigInt=0;JDConv=0;PWD=</v>
       </c>
@@ -3346,7 +3346,7 @@
       <c s="1" t="s">
         <v>65</v>
       </c>
-      <c s="5" t="str">
+      <c s="6" t="str">
         <f t="shared" si="0"/>
         <v>DSN=Flights;Database=C:\Users\somone\AppData\Local\UFT\Demo\DB\Flights.s3db;StepAPI=0;SyncPragma=;NoTXN=0;Timeout=;ShortNames=0;LongNames=0;NoCreat=0;NoWCHAR=0;FKSupport=0;JournalMode=;OEMCP=0;LoadExt=;BigInt=0;JDConv=0;PWD=</v>
       </c>
@@ -3355,7 +3355,7 @@
       <c s="1" t="s">
         <v>65</v>
       </c>
-      <c s="5" t="str">
+      <c s="6" t="str">
         <f t="shared" si="0"/>
         <v>DSN=Flights;Database=C:\Users\somone\AppData\Local\UFT\Demo\DB\Flights.s3db;StepAPI=0;SyncPragma=;NoTXN=0;Timeout=;ShortNames=0;LongNames=0;NoCreat=0;NoWCHAR=0;FKSupport=0;JournalMode=;OEMCP=0;LoadExt=;BigInt=0;JDConv=0;PWD=</v>
       </c>

</xml_diff>